<commit_message>
Development updates, task emails
</commit_message>
<xml_diff>
--- a/Processes/HR_FixedTermAppointmentExpiry/Data/Config.xlsx
+++ b/Processes/HR_FixedTermAppointmentExpiry/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CCD2083-DCC4-455D-9597-9947DD2D157F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B53DE8A1-6C04-4BB8-AE5F-BDD16440110A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4710" yWindow="2520" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="67">
   <si>
     <t>Name</t>
   </si>
@@ -211,6 +211,18 @@
   </si>
   <si>
     <t>Sets Robot to server type: Dev, Test, Staging or Prod</t>
+  </si>
+  <si>
+    <t>UQ_SMTP_SERVER</t>
+  </si>
+  <si>
+    <t>SMTP Server Address</t>
+  </si>
+  <si>
+    <t>UQ_SMTP_PORT</t>
+  </si>
+  <si>
+    <t>SMTP Server Port</t>
   </si>
 </sst>
 </file>
@@ -2852,9 +2864,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2950,8 +2960,28 @@
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C8" t="s">
+        <v>66</v>
+      </c>
+    </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Development update, code cleanup
</commit_message>
<xml_diff>
--- a/Processes/HR_FixedTermAppointmentExpiry/Data/Config.xlsx
+++ b/Processes/HR_FixedTermAppointmentExpiry/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B53DE8A1-6C04-4BB8-AE5F-BDD16440110A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98765201-7FAF-485C-B20C-081C3288CE7F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="73">
   <si>
     <t>Name</t>
   </si>
@@ -223,6 +223,24 @@
   </si>
   <si>
     <t>SMTP Server Port</t>
+  </si>
+  <si>
+    <t>HR_FTAE_SummaryEmailAddress</t>
+  </si>
+  <si>
+    <t>SummaryEmailAddress</t>
+  </si>
+  <si>
+    <t>Email address for FTAE summary</t>
+  </si>
+  <si>
+    <t>HR_FTAE_DevTestEmailAddress</t>
+  </si>
+  <si>
+    <t>DevTestEmailAddress</t>
+  </si>
+  <si>
+    <t>Email address for Dev and Test</t>
   </si>
 </sst>
 </file>
@@ -262,9 +280,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2862,9 +2883,12 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9:B10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2982,8 +3006,28 @@
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>68</v>
+      </c>
+      <c r="B9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10" t="s">
+        <v>72</v>
+      </c>
+    </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Development updates, retries for Aurion selectors, additional logging
</commit_message>
<xml_diff>
--- a/Processes/HR_FixedTermAppointmentExpiry/Data/Config.xlsx
+++ b/Processes/HR_FixedTermAppointmentExpiry/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98765201-7FAF-485C-B20C-081C3288CE7F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04201838-ED30-4797-B687-CAA7918742F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2565" yWindow="2430" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="76">
   <si>
     <t>Name</t>
   </si>
@@ -241,6 +241,15 @@
   </si>
   <si>
     <t>Email address for Dev and Test</t>
+  </si>
+  <si>
+    <t>HR_FTAE_AurionLink</t>
+  </si>
+  <si>
+    <t>Shortcut link to start Aurion</t>
+  </si>
+  <si>
+    <t>AurionLink</t>
   </si>
 </sst>
 </file>
@@ -2887,7 +2896,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:B10"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3028,7 +3037,17 @@
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>75</v>
+      </c>
+      <c r="B11" t="s">
+        <v>73</v>
+      </c>
+      <c r="C11" t="s">
+        <v>74</v>
+      </c>
+    </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Development updates, removed pay points, added PST name
</commit_message>
<xml_diff>
--- a/Processes/HR_FixedTermAppointmentExpiry/Data/Config.xlsx
+++ b/Processes/HR_FixedTermAppointmentExpiry/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Desktop\UQ FTAE Work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04201838-ED30-4797-B687-CAA7918742F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CF1C13F-D061-4CE7-810C-57682E05CE2B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2565" yWindow="2430" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="73">
   <si>
     <t>Name</t>
   </si>
@@ -198,15 +198,6 @@
     <t>T drive mapping for Aurion application</t>
   </si>
   <si>
-    <t>HR_FTAE_Aurion_PayPoint_FilePath</t>
-  </si>
-  <si>
-    <t>PayPointFile</t>
-  </si>
-  <si>
-    <t>File to match Pay Point Code to Pay Point Admin</t>
-  </si>
-  <si>
     <t>OperatingEnvironment</t>
   </si>
   <si>
@@ -234,15 +225,6 @@
     <t>Email address for FTAE summary</t>
   </si>
   <si>
-    <t>HR_FTAE_DevTestEmailAddress</t>
-  </si>
-  <si>
-    <t>DevTestEmailAddress</t>
-  </si>
-  <si>
-    <t>Email address for Dev and Test</t>
-  </si>
-  <si>
     <t>HR_FTAE_AurionLink</t>
   </si>
   <si>
@@ -250,6 +232,15 @@
   </si>
   <si>
     <t>AurionLink</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HR_FTAE_DefaultTaskEmailAddress    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DefaultTaskEmailAddress    </t>
+  </si>
+  <si>
+    <t>Email address for task if no PST match found</t>
   </si>
 </sst>
 </file>
@@ -2893,10 +2884,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2940,114 +2931,104 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C2" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
       <c r="B4" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="C4" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>59</v>
-      </c>
-      <c r="B5" t="s">
-        <v>58</v>
+      <c r="A5" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>70</v>
       </c>
       <c r="C5" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B6" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C6" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="B7" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="C7" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="B8" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="C8" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B9" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C9" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>70</v>
+      <c r="A10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" t="s">
+        <v>60</v>
       </c>
       <c r="C10" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>75</v>
-      </c>
-      <c r="B11" t="s">
-        <v>73</v>
-      </c>
-      <c r="C11" t="s">
-        <v>74</v>
-      </c>
-    </row>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4036,8 +4017,10 @@
     <row r="997" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="998" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="999" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C1001">
+    <sortCondition ref="B2:B1001"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Development updates, API retrofit
</commit_message>
<xml_diff>
--- a/Processes/HR_FixedTermAppointmentExpiry/Data/Config.xlsx
+++ b/Processes/HR_FixedTermAppointmentExpiry/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Desktop\UQ FTAE Work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CF1C13F-D061-4CE7-810C-57682E05CE2B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{920F3507-0B39-4DC1-8262-8F6C0C1FB12C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -234,13 +234,13 @@
     <t>AurionLink</t>
   </si>
   <si>
-    <t xml:space="preserve">HR_FTAE_DefaultTaskEmailAddress    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">DefaultTaskEmailAddress    </t>
-  </si>
-  <si>
     <t>Email address for task if no PST match found</t>
+  </si>
+  <si>
+    <t>HR_FTAE_DefaultTaskEmailAddress</t>
+  </si>
+  <si>
+    <t>DefaultTaskEmailAddress</t>
   </si>
 </sst>
 </file>
@@ -2886,9 +2886,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2964,13 +2962,13 @@
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" t="s">
         <v>70</v>
-      </c>
-      <c r="C5" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Development updates, API retrofit completed
</commit_message>
<xml_diff>
--- a/Processes/HR_FixedTermAppointmentExpiry/Data/Config.xlsx
+++ b/Processes/HR_FixedTermAppointmentExpiry/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Desktop\UQ FTAE Work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{920F3507-0B39-4DC1-8262-8F6C0C1FB12C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4B17A7C-A2CE-47A1-AE28-E89DD7256DF8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="76">
   <si>
     <t>Name</t>
   </si>
@@ -241,6 +241,15 @@
   </si>
   <si>
     <t>DefaultTaskEmailAddress</t>
+  </si>
+  <si>
+    <t>HR_FTAE_DevTestEmailAddress</t>
+  </si>
+  <si>
+    <t>DevTestEmailAddress</t>
+  </si>
+  <si>
+    <t>SMTP Server Address for dev and test</t>
   </si>
 </sst>
 </file>
@@ -3026,7 +3035,17 @@
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>74</v>
+      </c>
+      <c r="B11" t="s">
+        <v>73</v>
+      </c>
+      <c r="C11" t="s">
+        <v>75</v>
+      </c>
+    </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Aurion drive mapping is now dynamic to accommodate changing drive letters and paths
</commit_message>
<xml_diff>
--- a/Processes/HR_FixedTermAppointmentExpiry/Data/Config.xlsx
+++ b/Processes/HR_FixedTermAppointmentExpiry/Data/Config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Desktop\UQ FTAE Work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4B17A7C-A2CE-47A1-AE28-E89DD7256DF8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B88CD5D-52B2-422A-BF02-85C7BC495F1E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="82">
   <si>
     <t>Name</t>
   </si>
@@ -180,24 +180,6 @@
     <t>HR_FixedTermAppointmentExpiry</t>
   </si>
   <si>
-    <t>HR_FTAE_Aurion_J_Drive_FilePath</t>
-  </si>
-  <si>
-    <t>HR_FTAE_Aurion_T_Drive_FilePath</t>
-  </si>
-  <si>
-    <t>Jdrive</t>
-  </si>
-  <si>
-    <t>Tdrive</t>
-  </si>
-  <si>
-    <t>J drive mapping for Aurion application</t>
-  </si>
-  <si>
-    <t>T drive mapping for Aurion application</t>
-  </si>
-  <si>
     <t>OperatingEnvironment</t>
   </si>
   <si>
@@ -250,6 +232,42 @@
   </si>
   <si>
     <t>SMTP Server Address for dev and test</t>
+  </si>
+  <si>
+    <t>HR_FTAE_Aurion_Drive1_DriveLetter</t>
+  </si>
+  <si>
+    <t>HR_FTAE_Aurion_Drive1_FilePath</t>
+  </si>
+  <si>
+    <t>HR_FTAE_Aurion_Drive2_DriveLetter</t>
+  </si>
+  <si>
+    <t>HR_FTAE_Aurion_Drive2_FilePath</t>
+  </si>
+  <si>
+    <t>Drive1_DriveLetter</t>
+  </si>
+  <si>
+    <t>Drive2_DriveLetter</t>
+  </si>
+  <si>
+    <t>Drive2_FilePath</t>
+  </si>
+  <si>
+    <t>Drive1_FilePath</t>
+  </si>
+  <si>
+    <t>Drive 1 drive letter for Aurion application</t>
+  </si>
+  <si>
+    <t>Drive 2 drive letter for Aurion application</t>
+  </si>
+  <si>
+    <t>Drive 1 file path for Aurion application</t>
+  </si>
+  <si>
+    <t>Drive 2 file path for Aurion application</t>
   </si>
 </sst>
 </file>
@@ -2893,9 +2911,11 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:Z999"/>
+  <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2938,116 +2958,136 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>54</v>
+        <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>52</v>
+        <v>70</v>
       </c>
       <c r="C2" t="s">
-        <v>56</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>55</v>
+        <v>77</v>
       </c>
       <c r="B3" t="s">
-        <v>53</v>
+        <v>71</v>
       </c>
       <c r="C3" t="s">
-        <v>57</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="B4" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="C4" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>71</v>
+      <c r="A5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B5" t="s">
+        <v>73</v>
       </c>
       <c r="C5" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C6" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>49</v>
-      </c>
-      <c r="B7" t="s">
-        <v>48</v>
+      <c r="A7" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>65</v>
       </c>
       <c r="C7" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B8" t="s">
         <v>58</v>
       </c>
       <c r="C8" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="B9" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="C9" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="B10" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="C10" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>74</v>
+        <v>56</v>
       </c>
       <c r="B11" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="C11" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>68</v>
+      </c>
+      <c r="B13" t="s">
+        <v>67</v>
+      </c>
+      <c r="C13" t="s">
+        <v>69</v>
+      </c>
+    </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4034,9 +4074,11 @@
     <row r="997" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="998" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="999" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1001" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C1001">
-    <sortCondition ref="B2:B1001"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C1003">
+    <sortCondition ref="B2:B1003"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added value for Prod UniTask to config.xlsx
</commit_message>
<xml_diff>
--- a/Processes/HR_FixedTermAppointmentExpiry/Data/Config.xlsx
+++ b/Processes/HR_FixedTermAppointmentExpiry/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Desktop\UQ FTAE Work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E2CD85E-60A0-42A7-A684-9DB00F718066}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88DAA8FF-5AA3-42C7-AEEA-1EB8C0F3BADD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="75" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="101">
   <si>
     <t>Name</t>
   </si>
@@ -322,13 +322,16 @@
   </si>
   <si>
     <t>UnitaskURL-PROD</t>
+  </si>
+  <si>
+    <t>https://unitask.uq.edu.au/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -339,6 +342,13 @@
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -358,17 +368,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1018,11 +1032,16 @@
       <c r="A35" t="s">
         <v>99</v>
       </c>
+      <c r="B35" s="4" t="s">
+        <v>100</v>
+      </c>
       <c r="C35" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="36" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="3"/>
+    </row>
     <row r="37" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="38" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="39" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1967,6 +1986,7 @@
     <row r="978" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updated Staging Unitask URL
</commit_message>
<xml_diff>
--- a/Processes/HR_FixedTermAppointmentExpiry/Data/Config.xlsx
+++ b/Processes/HR_FixedTermAppointmentExpiry/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Desktop\UQ FTAE Work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88DAA8FF-5AA3-42C7-AEEA-1EB8C0F3BADD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA608830-6FDF-4D44-994C-D5AFE3A8D37C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="75" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="102">
   <si>
     <t>Name</t>
   </si>
@@ -325,6 +325,9 @@
   </si>
   <si>
     <t>https://unitask.uq.edu.au/</t>
+  </si>
+  <si>
+    <t>https://task-staging.bpd.aws.uq.edu.au/</t>
   </si>
 </sst>
 </file>
@@ -697,7 +700,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z978"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -980,8 +985,8 @@
       <c r="A28" t="s">
         <v>93</v>
       </c>
-      <c r="B28" t="s">
-        <v>79</v>
+      <c r="B28" s="4" t="s">
+        <v>101</v>
       </c>
       <c r="C28" t="s">
         <v>48</v>

</xml_diff>

<commit_message>
Updated config.xlsx to correct Unitask URLs
</commit_message>
<xml_diff>
--- a/Processes/HR_FixedTermAppointmentExpiry/Data/Config.xlsx
+++ b/Processes/HR_FixedTermAppointmentExpiry/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Desktop\UQ FTAE Work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA608830-6FDF-4D44-994C-D5AFE3A8D37C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8417F847-2596-47D2-9212-CBACA6E04CDD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="75" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -324,10 +324,10 @@
     <t>UnitaskURL-PROD</t>
   </si>
   <si>
-    <t>https://unitask.uq.edu.au/</t>
-  </si>
-  <si>
-    <t>https://task-staging.bpd.aws.uq.edu.au/</t>
+    <t>https://task-staging.bpd.aws.uq.edu.au</t>
+  </si>
+  <si>
+    <t>https://unitask.uq.edu.au</t>
   </si>
 </sst>
 </file>
@@ -701,7 +701,7 @@
   <dimension ref="A1:Z978"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -785,7 +785,7 @@
       <c r="A7" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="4" t="s">
         <v>81</v>
       </c>
       <c r="C7" t="s">
@@ -986,7 +986,7 @@
         <v>93</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C28" t="s">
         <v>48</v>
@@ -1038,7 +1038,7 @@
         <v>99</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C35" t="s">
         <v>48</v>

</xml_diff>

<commit_message>
Config updated with Prod Aurion details, commented out code removed
</commit_message>
<xml_diff>
--- a/Processes/HR_FixedTermAppointmentExpiry/Data/Config.xlsx
+++ b/Processes/HR_FixedTermAppointmentExpiry/Data/Config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Desktop\UQ FTAE Work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8417F847-2596-47D2-9212-CBACA6E04CDD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8589F140-050A-403D-891F-D737C53442BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="75" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="107">
   <si>
     <t>Name</t>
   </si>
@@ -328,6 +328,21 @@
   </si>
   <si>
     <t>https://unitask.uq.edu.au</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>\\nas01.storage.uq.edu.au\aur_prod</t>
+  </si>
+  <si>
+    <t>\\nas01.storage.uq.edu.au\aurion11_prod</t>
+  </si>
+  <si>
+    <t>Q:\Shortcuts\AURPROD RPA urouter.lnk</t>
   </si>
 </sst>
 </file>
@@ -375,7 +390,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -383,6 +398,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -700,9 +716,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z978"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -997,6 +1011,9 @@
       <c r="A30" t="s">
         <v>94</v>
       </c>
+      <c r="B30" t="s">
+        <v>102</v>
+      </c>
       <c r="C30" t="s">
         <v>64</v>
       </c>
@@ -1005,6 +1022,9 @@
       <c r="A31" t="s">
         <v>95</v>
       </c>
+      <c r="B31" s="4" t="s">
+        <v>104</v>
+      </c>
       <c r="C31" t="s">
         <v>66</v>
       </c>
@@ -1013,6 +1033,9 @@
       <c r="A32" t="s">
         <v>96</v>
       </c>
+      <c r="B32" s="5" t="s">
+        <v>103</v>
+      </c>
       <c r="C32" t="s">
         <v>65</v>
       </c>
@@ -1021,6 +1044,9 @@
       <c r="A33" t="s">
         <v>97</v>
       </c>
+      <c r="B33" s="4" t="s">
+        <v>105</v>
+      </c>
       <c r="C33" t="s">
         <v>67</v>
       </c>
@@ -1028,6 +1054,9 @@
     <row r="34" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>98</v>
+      </c>
+      <c r="B34" t="s">
+        <v>106</v>
       </c>
       <c r="C34" t="s">
         <v>59</v>

</xml_diff>

<commit_message>
Updated dev email address
</commit_message>
<xml_diff>
--- a/Processes/HR_FixedTermAppointmentExpiry/Data/Config.xlsx
+++ b/Processes/HR_FixedTermAppointmentExpiry/Data/Config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Desktop\UQ FTAE Work\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8589F140-050A-403D-891F-D737C53442BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B835C3E-F175-451A-BA7E-8AA170C0CF70}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="75" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -264,9 +264,6 @@
     <t>https://task-test.bpd.aws.uq.edu.au</t>
   </si>
   <si>
-    <t>s.debbe@uq.edu.au; s.gururaj@uq.edu.au</t>
-  </si>
-  <si>
     <t>employeeservices.hr@enquire.uq.edu.au</t>
   </si>
   <si>
@@ -343,6 +340,9 @@
   </si>
   <si>
     <t>Q:\Shortcuts\AURPROD RPA urouter.lnk</t>
+  </si>
+  <si>
+    <t>s.debbe@uq.edu.au</t>
   </si>
 </sst>
 </file>
@@ -716,7 +716,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z978"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -788,8 +790,8 @@
       <c r="A6" t="s">
         <v>62</v>
       </c>
-      <c r="B6" t="s">
-        <v>80</v>
+      <c r="B6" s="4" t="s">
+        <v>106</v>
       </c>
       <c r="C6" t="s">
         <v>63</v>
@@ -800,7 +802,7 @@
         <v>61</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C7" t="s">
         <v>60</v>
@@ -876,7 +878,7 @@
     <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B16" t="s">
         <v>73</v>
@@ -887,7 +889,7 @@
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B17" t="s">
         <v>74</v>
@@ -898,7 +900,7 @@
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B18" t="s">
         <v>76</v>
@@ -909,7 +911,7 @@
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B19" t="s">
         <v>77</v>
@@ -920,7 +922,7 @@
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B20" t="s">
         <v>78</v>
@@ -931,7 +933,7 @@
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B21" t="s">
         <v>79</v>
@@ -942,7 +944,7 @@
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B23" t="s">
         <v>73</v>
@@ -953,7 +955,7 @@
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B24" t="s">
         <v>74</v>
@@ -964,7 +966,7 @@
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B25" t="s">
         <v>76</v>
@@ -975,7 +977,7 @@
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B26" t="s">
         <v>77</v>
@@ -986,7 +988,7 @@
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B27" t="s">
         <v>78</v>
@@ -997,10 +999,10 @@
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C28" t="s">
         <v>48</v>
@@ -1009,10 +1011,10 @@
     <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B30" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C30" t="s">
         <v>64</v>
@@ -1020,10 +1022,10 @@
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C31" t="s">
         <v>66</v>
@@ -1031,10 +1033,10 @@
     </row>
     <row r="32" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C32" t="s">
         <v>65</v>
@@ -1042,10 +1044,10 @@
     </row>
     <row r="33" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C33" t="s">
         <v>67</v>
@@ -1053,10 +1055,10 @@
     </row>
     <row r="34" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B34" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C34" t="s">
         <v>59</v>
@@ -1064,10 +1066,10 @@
     </row>
     <row r="35" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C35" t="s">
         <v>48</v>

</xml_diff>

<commit_message>
Aurion disabled pop up
</commit_message>
<xml_diff>
--- a/Processes/HR_FixedTermAppointmentExpiry/Data/Config.xlsx
+++ b/Processes/HR_FixedTermAppointmentExpiry/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B835C3E-F175-451A-BA7E-8AA170C0CF70}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2EA28ED-23A7-4923-9C3E-D6BA31EB9C7E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="75" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -258,9 +258,6 @@
     <t>\\nas01.storage.uq.edu.au\aur_xtrn</t>
   </si>
   <si>
-    <t>Z:\Shortcuts\Aurion 11 AURXTRN urouter.lnk</t>
-  </si>
-  <si>
     <t>https://task-test.bpd.aws.uq.edu.au</t>
   </si>
   <si>
@@ -343,6 +340,9 @@
   </si>
   <si>
     <t>s.debbe@uq.edu.au</t>
+  </si>
+  <si>
+    <t>Z:\Shortcuts\Aurion 11 AURXTRN RPA urouter.lnk</t>
   </si>
 </sst>
 </file>
@@ -716,9 +716,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z978"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -791,7 +789,7 @@
         <v>62</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C6" t="s">
         <v>63</v>
@@ -802,7 +800,7 @@
         <v>61</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C7" t="s">
         <v>60</v>
@@ -858,7 +856,7 @@
         <v>71</v>
       </c>
       <c r="B13" t="s">
-        <v>78</v>
+        <v>106</v>
       </c>
       <c r="C13" t="s">
         <v>59</v>
@@ -869,7 +867,7 @@
         <v>72</v>
       </c>
       <c r="B14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C14" t="s">
         <v>48</v>
@@ -878,7 +876,7 @@
     <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B16" t="s">
         <v>73</v>
@@ -889,7 +887,7 @@
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B17" t="s">
         <v>74</v>
@@ -900,7 +898,7 @@
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B18" t="s">
         <v>76</v>
@@ -911,7 +909,7 @@
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B19" t="s">
         <v>77</v>
@@ -922,10 +920,10 @@
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B20" t="s">
-        <v>78</v>
+        <v>106</v>
       </c>
       <c r="C20" t="s">
         <v>59</v>
@@ -933,10 +931,10 @@
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B21" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C21" t="s">
         <v>48</v>
@@ -944,7 +942,7 @@
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B23" t="s">
         <v>73</v>
@@ -955,7 +953,7 @@
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B24" t="s">
         <v>74</v>
@@ -966,7 +964,7 @@
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B25" t="s">
         <v>76</v>
@@ -977,7 +975,7 @@
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B26" t="s">
         <v>77</v>
@@ -988,10 +986,10 @@
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B27" t="s">
-        <v>78</v>
+        <v>106</v>
       </c>
       <c r="C27" t="s">
         <v>59</v>
@@ -999,10 +997,10 @@
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C28" t="s">
         <v>48</v>
@@ -1011,10 +1009,10 @@
     <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B30" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C30" t="s">
         <v>64</v>
@@ -1022,10 +1020,10 @@
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C31" t="s">
         <v>66</v>
@@ -1033,10 +1031,10 @@
     </row>
     <row r="32" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C32" t="s">
         <v>65</v>
@@ -1044,10 +1042,10 @@
     </row>
     <row r="33" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C33" t="s">
         <v>67</v>
@@ -1055,10 +1053,10 @@
     </row>
     <row r="34" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B34" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C34" t="s">
         <v>59</v>
@@ -1066,10 +1064,10 @@
     </row>
     <row r="35" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C35" t="s">
         <v>48</v>

</xml_diff>